<commit_message>
switch to "Corrected Current Volume (uL)"
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_v5_3_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_v5_3_0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="449">
   <si>
     <t xml:space="preserve">Sample Transfer Template</t>
   </si>
@@ -101,70 +101,73 @@
     <t xml:space="preserve">Current Volume (uL)</t>
   </si>
   <si>
+    <t xml:space="preserve">Corrected Current Volume (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Used (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer Date (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workflow Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Transfer template instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample transfer template moves a volume of sample from one container to another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the "Destination Container Coord" is set to "Yes" the destination coordinates will be set to the source coordinates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details on fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample name of the source of the transfer. This is used for validation purpose to confirm the expected sample matches the container location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique barcode of the container holding the source sample.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinate of the source sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique barcode of the container holding the transfered sample.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinate of the transfered sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the destination container. The name only needs to be provided when a new container is defined, otherwise the barcode is sufficient.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kind of the destination container. The kind only needs to be provided when a new container is defined, otherwise the barcode is sufficient.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique barcode of the container holding the destination container.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinate of the destination container within the parent container. Using the alphanumerical coordinates names (e.g. A01).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Force the depletion status of the source sample even if the volume is not zero. The source sample volume will not be affected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current volume value in uL stored in freezeman at the time of the prefilling. Used as an indicative value to facilitate template completion.</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Current Volume (uL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume Used (uL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transfer Date (YYYY-MM-DD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination Study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workflow Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Transfer template instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample transfer template moves a volume of sample from one container to another.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the "Destination Container Coord" is set to "Yes" the destination coordinates will be set to the source coordinates.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details on fields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample name of the source of the transfer. This is used for validation purpose to confirm the expected sample matches the container location.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique barcode of the container holding the source sample.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinate of the source sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique barcode of the container holding the transfered sample.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinate of the transfered sample within the container. Using the alphanumerical coordinates names (e.g. A01).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of the destination container. The name only needs to be provided when a new container is defined, otherwise the barcode is sufficient.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kind of the destination container. The kind only needs to be provided when a new container is defined, otherwise the barcode is sufficient.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique barcode of the container holding the destination container.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinate of the destination container within the parent container. Using the alphanumerical coordinates names (e.g. A01).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Force the depletion status of the source sample even if the volume is not zero. The source sample volume will not be affected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current volume value in uL stored in freezeman at the time of the prefilling. Used as an indicative value to facilitate template completion.</t>
   </si>
   <si>
     <t xml:space="preserve">Volume value in uL of the source sample right before the transfer including additional volume used for dilution.</t>
@@ -2131,7 +2134,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="38.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="21.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="38.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="34.83"/>
@@ -12115,10 +12119,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="44" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="4"/>
@@ -12146,7 +12150,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" s="46"/>
       <c r="D20" s="4"/>
@@ -12174,7 +12178,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" s="46"/>
       <c r="D21" s="4"/>
@@ -12202,7 +12206,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C22" s="46"/>
       <c r="D22" s="4"/>
@@ -12230,7 +12234,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" s="46"/>
       <c r="D23" s="4"/>
@@ -12258,7 +12262,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="46"/>
       <c r="D24" s="4"/>
@@ -12286,7 +12290,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -12932,13 +12936,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>22</v>
@@ -12949,2261 +12953,2261 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B202" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B203" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B204" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B205" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B206" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B207" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B208" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B209" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B210" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B211" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B212" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B213" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B214" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B215" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B216" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B217" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B218" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B219" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B220" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B221" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B222" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B223" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B224" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B225" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B226" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B227" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B228" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B229" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B230" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B231" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B232" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B233" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B234" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B235" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B236" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B237" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B238" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B239" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B240" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B241" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B245" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B246" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B248" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B249" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B250" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B251" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B252" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B253" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B254" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B255" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B256" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B257" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B258" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B259" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B260" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B261" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B262" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B263" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B264" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B265" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B266" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B267" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B268" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B269" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B270" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B271" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B272" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B273" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B274" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B275" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B276" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B277" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B278" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B279" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B280" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B281" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B282" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B283" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B284" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B285" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B286" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B287" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B288" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B289" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B290" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B291" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B292" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B293" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B294" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B295" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B296" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B297" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B298" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B299" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B300" s="4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B303" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B304" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B305" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B306" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B307" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B308" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B309" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B310" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B311" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B312" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B313" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B314" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B315" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B316" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B317" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B318" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B319" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B320" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B321" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B322" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B323" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B324" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B325" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B326" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B327" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B328" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B329" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B330" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B331" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B332" s="4" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B333" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B334" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B335" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B336" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B337" s="4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B338" s="4" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B339" s="4" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B340" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B341" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B342" s="4" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B343" s="4" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B344" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B345" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B346" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B347" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B348" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B349" s="4" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B350" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B351" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B352" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B353" s="4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B354" s="4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B355" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B356" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B357" s="4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B358" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B359" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B360" s="4" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B361" s="4" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B362" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B363" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B364" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B365" s="4" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B366" s="4" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B367" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B368" s="4" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B369" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B370" s="4" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B371" s="4" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B372" s="4" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B373" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B374" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B375" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B376" s="4" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B377" s="4" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B378" s="4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B379" s="4" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B380" s="4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B381" s="4" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B382" s="4" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B383" s="4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B384" s="4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B385" s="4" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
tweaks based on @UlysseFG
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_v5_3_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_v5_3_0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="448">
   <si>
     <t xml:space="preserve">Sample Transfer Template</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t xml:space="preserve">Current volume value in uL stored in freezeman at the time of the prefilling. Used as an indicative value to facilitate template completion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Current Volume (uL)</t>
   </si>
   <si>
     <t xml:space="preserve">Volume value in uL of the source sample right before the transfer including additional volume used for dilution.</t>
@@ -2134,7 +2131,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="38.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="29.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="38.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="55"/>
@@ -12119,10 +12116,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="45" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>39</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="4"/>
@@ -12150,7 +12147,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="46"/>
       <c r="D20" s="4"/>
@@ -12178,7 +12175,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="46"/>
       <c r="D21" s="4"/>
@@ -12206,7 +12203,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="46"/>
       <c r="D22" s="4"/>
@@ -12234,7 +12231,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="46"/>
       <c r="D23" s="4"/>
@@ -12262,7 +12259,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="46"/>
       <c r="D24" s="4"/>
@@ -12290,7 +12287,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -12936,13 +12933,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>22</v>
@@ -12953,2261 +12950,2261 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B92" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B94" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B96" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B202" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B203" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B204" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B205" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B206" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B207" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B208" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B209" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B210" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B211" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B212" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B213" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B214" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B215" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B216" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B217" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B218" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B219" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B220" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B221" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B222" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B223" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B224" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B225" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B226" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B227" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B228" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B229" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B230" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B231" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B232" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B233" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B234" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B235" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B236" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B237" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B238" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B239" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B240" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B241" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B245" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B246" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B248" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B249" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B250" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B251" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B252" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B253" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B254" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B255" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B256" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B257" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B258" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B259" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B260" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B261" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B262" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B263" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B264" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B265" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B266" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B267" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B268" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B269" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B270" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B271" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B272" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B273" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B274" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B275" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B276" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B277" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B278" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B279" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B280" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B281" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B282" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B283" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B284" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B285" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B286" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B287" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B288" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B289" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B290" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B291" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B292" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B293" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B294" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B295" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B296" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B297" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B298" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B299" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B300" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B303" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B304" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B305" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B306" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B307" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B308" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B309" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B310" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B311" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B312" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B313" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B314" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B315" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B316" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B317" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B318" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B319" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B320" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B321" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B322" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B323" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B324" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B325" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B326" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B327" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B328" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B329" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B330" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B331" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B332" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B333" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B334" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B335" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B336" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B337" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B338" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B339" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B340" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B341" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B342" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B343" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B344" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B345" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B346" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B347" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B348" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B349" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B350" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B351" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B352" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B353" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B354" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B355" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B356" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B357" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B358" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B359" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B360" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B361" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B362" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B363" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B364" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B365" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B366" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B367" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B368" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B369" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B370" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B371" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B372" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B373" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B374" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B375" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B376" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B377" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B378" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B379" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B380" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B381" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B382" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B383" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B384" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B385" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>